<commit_message>
Terminado + licencia + read.me
</commit_message>
<xml_diff>
--- a/FaceBook/model_FB.xlsx
+++ b/FaceBook/model_FB.xlsx
@@ -462,12 +462,12 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -477,7 +477,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -502,12 +502,12 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -517,17 +517,17 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -537,47 +537,47 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30">
@@ -587,7 +587,7 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
@@ -622,22 +622,22 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
@@ -647,7 +647,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
@@ -657,17 +657,17 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
@@ -682,7 +682,7 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51">
@@ -692,22 +692,22 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56">
@@ -717,7 +717,7 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
@@ -727,82 +727,82 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
@@ -817,7 +817,7 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78">
@@ -827,22 +827,22 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83">
@@ -857,27 +857,27 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90">
@@ -892,7 +892,7 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93">
@@ -907,22 +907,22 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99">
@@ -947,7 +947,7 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104">
@@ -957,7 +957,7 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106">
@@ -967,12 +967,12 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109">
@@ -1002,12 +1002,12 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116">
@@ -1027,17 +1027,17 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122">
@@ -1047,7 +1047,7 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124">
@@ -1057,12 +1057,12 @@
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127">
@@ -1072,7 +1072,7 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129">
@@ -1082,7 +1082,7 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131">
@@ -1102,17 +1102,17 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137">
@@ -1122,7 +1122,7 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139">
@@ -1137,12 +1137,12 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143">
@@ -1152,17 +1152,17 @@
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="147">
@@ -1182,12 +1182,12 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="152">
@@ -1202,7 +1202,7 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="155">
@@ -1212,17 +1212,17 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="159">
@@ -1232,7 +1232,7 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161">
@@ -1252,7 +1252,7 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165">
@@ -1272,7 +1272,7 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169">
@@ -1287,17 +1287,17 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174">
@@ -1307,7 +1307,7 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="176">
@@ -1332,7 +1332,7 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="181">
@@ -1342,17 +1342,17 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="185">
@@ -1367,17 +1367,17 @@
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="190">
@@ -1387,22 +1387,22 @@
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195">
@@ -1427,7 +1427,7 @@
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="200">
@@ -1437,7 +1437,7 @@
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="202">
@@ -1447,17 +1447,17 @@
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="206">
@@ -1477,27 +1477,27 @@
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="214">
@@ -1507,17 +1507,17 @@
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="218">
@@ -1527,42 +1527,42 @@
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="227">
@@ -1572,12 +1572,12 @@
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="230">
@@ -1592,7 +1592,7 @@
     </row>
     <row r="232">
       <c r="A232" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="233">
@@ -1602,27 +1602,27 @@
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="239">
@@ -1647,17 +1647,17 @@
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="246">
@@ -1667,7 +1667,7 @@
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="248">
@@ -1692,7 +1692,7 @@
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="253">
@@ -1702,7 +1702,7 @@
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="255">
@@ -1712,37 +1712,37 @@
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="263">
@@ -1752,7 +1752,7 @@
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="265">
@@ -1762,12 +1762,12 @@
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="268">
@@ -1787,7 +1787,7 @@
     </row>
     <row r="271">
       <c r="A271" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="272">
@@ -1797,32 +1797,32 @@
     </row>
     <row r="273">
       <c r="A273" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="279">
@@ -1832,47 +1832,47 @@
     </row>
     <row r="280">
       <c r="A280" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="289">
@@ -1882,17 +1882,17 @@
     </row>
     <row r="290">
       <c r="A290" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="293">
@@ -1907,27 +1907,27 @@
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="300">
@@ -1937,7 +1937,7 @@
     </row>
     <row r="301">
       <c r="A301" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="302">
@@ -1957,62 +1957,62 @@
     </row>
     <row r="305">
       <c r="A305" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="317">
@@ -2022,7 +2022,7 @@
     </row>
     <row r="318">
       <c r="A318" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="319">
@@ -2032,12 +2032,12 @@
     </row>
     <row r="320">
       <c r="A320" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="322">
@@ -2047,7 +2047,7 @@
     </row>
     <row r="323">
       <c r="A323" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="324">
@@ -2057,27 +2057,27 @@
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="330">
@@ -2087,7 +2087,7 @@
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="332">
@@ -2097,22 +2097,22 @@
     </row>
     <row r="333">
       <c r="A333" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="337">
@@ -2127,12 +2127,12 @@
     </row>
     <row r="339">
       <c r="A339" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="341">
@@ -2147,17 +2147,17 @@
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="346">
@@ -2182,22 +2182,22 @@
     </row>
     <row r="350">
       <c r="A350" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="354">
@@ -2207,12 +2207,12 @@
     </row>
     <row r="355">
       <c r="A355" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="357">
@@ -2222,22 +2222,22 @@
     </row>
     <row r="358">
       <c r="A358" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="362">
@@ -2247,32 +2247,32 @@
     </row>
     <row r="363">
       <c r="A363" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="369">
@@ -2282,7 +2282,7 @@
     </row>
     <row r="370">
       <c r="A370" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="371">
@@ -2292,7 +2292,7 @@
     </row>
     <row r="372">
       <c r="A372" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="373">
@@ -2312,12 +2312,12 @@
     </row>
     <row r="376">
       <c r="A376" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="378">
@@ -2327,7 +2327,7 @@
     </row>
     <row r="379">
       <c r="A379" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="380">
@@ -2337,7 +2337,7 @@
     </row>
     <row r="381">
       <c r="A381" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="382">
@@ -2357,7 +2357,7 @@
     </row>
     <row r="385">
       <c r="A385" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="386">
@@ -2372,42 +2372,42 @@
     </row>
     <row r="388">
       <c r="A388" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="396">
@@ -2422,22 +2422,22 @@
     </row>
     <row r="398">
       <c r="A398" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="402">
@@ -2447,22 +2447,22 @@
     </row>
     <row r="403">
       <c r="A403" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="407">
@@ -2477,12 +2477,12 @@
     </row>
     <row r="409">
       <c r="A409" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="411">
@@ -2492,7 +2492,7 @@
     </row>
     <row r="412">
       <c r="A412" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="413">
@@ -2502,17 +2502,17 @@
     </row>
     <row r="414">
       <c r="A414" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="417">
@@ -2532,17 +2532,17 @@
     </row>
     <row r="420">
       <c r="A420" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="423">
@@ -2557,22 +2557,22 @@
     </row>
     <row r="425">
       <c r="A425" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="429">
@@ -2587,17 +2587,17 @@
     </row>
     <row r="431">
       <c r="A431" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="434">
@@ -2607,27 +2607,27 @@
     </row>
     <row r="435">
       <c r="A435" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="440">
@@ -2642,7 +2642,7 @@
     </row>
     <row r="442">
       <c r="A442" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="443">
@@ -2667,37 +2667,37 @@
     </row>
     <row r="447">
       <c r="A447" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="454">
@@ -2707,27 +2707,27 @@
     </row>
     <row r="455">
       <c r="A455" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="460">
@@ -2737,17 +2737,17 @@
     </row>
     <row r="461">
       <c r="A461" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="464">
@@ -2757,27 +2757,27 @@
     </row>
     <row r="465">
       <c r="A465" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="470">
@@ -2787,12 +2787,12 @@
     </row>
     <row r="471">
       <c r="A471" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="472">
       <c r="A472" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="473">
@@ -2802,12 +2802,12 @@
     </row>
     <row r="474">
       <c r="A474" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="476">
@@ -2817,22 +2817,22 @@
     </row>
     <row r="477">
       <c r="A477" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="478">
       <c r="A478" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="479">
       <c r="A479" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="480">
       <c r="A480" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="481">
@@ -2842,7 +2842,7 @@
     </row>
     <row r="482">
       <c r="A482" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="483">
@@ -2852,7 +2852,7 @@
     </row>
     <row r="484">
       <c r="A484" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="485">
@@ -2862,7 +2862,7 @@
     </row>
     <row r="486">
       <c r="A486" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="487">
@@ -2877,7 +2877,7 @@
     </row>
     <row r="489">
       <c r="A489" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="490">
@@ -2892,12 +2892,12 @@
     </row>
     <row r="492">
       <c r="A492" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="494">
@@ -2912,7 +2912,7 @@
     </row>
     <row r="496">
       <c r="A496" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="497">
@@ -2927,7 +2927,7 @@
     </row>
     <row r="499">
       <c r="A499" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="500">
@@ -2937,12 +2937,12 @@
     </row>
     <row r="501">
       <c r="A501" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="502">
       <c r="A502" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="503">
@@ -2952,12 +2952,12 @@
     </row>
     <row r="504">
       <c r="A504" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="505">
       <c r="A505" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="506">
@@ -2972,12 +2972,12 @@
     </row>
     <row r="508">
       <c r="A508" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="509">
       <c r="A509" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="510">
@@ -2992,7 +2992,7 @@
     </row>
     <row r="512">
       <c r="A512" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="513">
@@ -3002,12 +3002,12 @@
     </row>
     <row r="514">
       <c r="A514" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="515">
       <c r="A515" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="516">
@@ -3017,7 +3017,7 @@
     </row>
     <row r="517">
       <c r="A517" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="518">
@@ -3027,57 +3027,57 @@
     </row>
     <row r="519">
       <c r="A519" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="520">
       <c r="A520" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="521">
       <c r="A521" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="522">
       <c r="A522" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="523">
       <c r="A523" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="524">
       <c r="A524" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="525">
       <c r="A525" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="526">
       <c r="A526" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="527">
       <c r="A527" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="528">
       <c r="A528" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="529">
       <c r="A529" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="530">
@@ -3087,7 +3087,7 @@
     </row>
     <row r="531">
       <c r="A531" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="532">
@@ -3107,7 +3107,7 @@
     </row>
     <row r="535">
       <c r="A535" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="536">
@@ -3122,12 +3122,12 @@
     </row>
     <row r="538">
       <c r="A538" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="539">
       <c r="A539" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="540">
@@ -3142,12 +3142,12 @@
     </row>
     <row r="542">
       <c r="A542" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="543">
       <c r="A543" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="544">
@@ -3172,12 +3172,12 @@
     </row>
     <row r="548">
       <c r="A548" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="549">
       <c r="A549" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="550">
@@ -3207,7 +3207,7 @@
     </row>
     <row r="555">
       <c r="A555" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="556">
@@ -3217,7 +3217,7 @@
     </row>
     <row r="557">
       <c r="A557" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="558">
@@ -3227,17 +3227,17 @@
     </row>
     <row r="559">
       <c r="A559" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="560">
       <c r="A560" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="561">
       <c r="A561" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="562">
@@ -3247,17 +3247,17 @@
     </row>
     <row r="563">
       <c r="A563" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="564">
       <c r="A564" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="565">
       <c r="A565" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="566">
@@ -3277,7 +3277,7 @@
     </row>
     <row r="569">
       <c r="A569" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="570">
@@ -3287,32 +3287,32 @@
     </row>
     <row r="571">
       <c r="A571" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="572">
       <c r="A572" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="573">
       <c r="A573" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="574">
       <c r="A574" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="575">
       <c r="A575" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="576">
       <c r="A576" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="577">
@@ -3322,7 +3322,7 @@
     </row>
     <row r="578">
       <c r="A578" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="579">
@@ -3337,12 +3337,12 @@
     </row>
     <row r="581">
       <c r="A581" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="582">
       <c r="A582" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="583">
@@ -3352,12 +3352,12 @@
     </row>
     <row r="584">
       <c r="A584" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="585">
       <c r="A585" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="586">
@@ -3367,7 +3367,7 @@
     </row>
     <row r="587">
       <c r="A587" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="588">
@@ -3382,12 +3382,12 @@
     </row>
     <row r="590">
       <c r="A590" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="591">
       <c r="A591" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="592">
@@ -3402,7 +3402,7 @@
     </row>
     <row r="594">
       <c r="A594" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="595">
@@ -3422,7 +3422,7 @@
     </row>
     <row r="598">
       <c r="A598" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="599">
@@ -3442,7 +3442,7 @@
     </row>
     <row r="602">
       <c r="A602" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="603">
@@ -3452,12 +3452,12 @@
     </row>
     <row r="604">
       <c r="A604" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="605">
       <c r="A605" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="606">
@@ -3472,12 +3472,12 @@
     </row>
     <row r="608">
       <c r="A608" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="609">
       <c r="A609" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="610">
@@ -3487,17 +3487,17 @@
     </row>
     <row r="611">
       <c r="A611" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="612">
       <c r="A612" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="613">
       <c r="A613" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="614">
@@ -3507,7 +3507,7 @@
     </row>
     <row r="615">
       <c r="A615" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="616">
@@ -3517,7 +3517,7 @@
     </row>
     <row r="617">
       <c r="A617" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="618">
@@ -3537,22 +3537,22 @@
     </row>
     <row r="621">
       <c r="A621" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="622">
       <c r="A622" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="623">
       <c r="A623" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="624">
       <c r="A624" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="625">
@@ -3562,7 +3562,7 @@
     </row>
     <row r="626">
       <c r="A626" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="627">
@@ -3572,12 +3572,12 @@
     </row>
     <row r="628">
       <c r="A628" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="629">
       <c r="A629" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="630">
@@ -3587,22 +3587,22 @@
     </row>
     <row r="631">
       <c r="A631" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="632">
       <c r="A632" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="633">
       <c r="A633" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="634">
       <c r="A634" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="635">
@@ -3632,7 +3632,7 @@
     </row>
     <row r="640">
       <c r="A640" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="641">
@@ -3642,12 +3642,12 @@
     </row>
     <row r="642">
       <c r="A642" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="643">
       <c r="A643" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="644">
@@ -3662,27 +3662,27 @@
     </row>
     <row r="646">
       <c r="A646" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="647">
       <c r="A647" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="648">
       <c r="A648" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="649">
       <c r="A649" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="650">
       <c r="A650" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="651">
@@ -3697,22 +3697,22 @@
     </row>
     <row r="653">
       <c r="A653" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="654">
       <c r="A654" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="655">
       <c r="A655" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="656">
       <c r="A656" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="657">
@@ -3732,7 +3732,7 @@
     </row>
     <row r="660">
       <c r="A660" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="661">
@@ -3772,12 +3772,12 @@
     </row>
     <row r="668">
       <c r="A668" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="669">
       <c r="A669" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="670">
@@ -3787,27 +3787,27 @@
     </row>
     <row r="671">
       <c r="A671" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="672">
       <c r="A672" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="673">
       <c r="A673" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="674">
       <c r="A674" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="675">
       <c r="A675" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="676">
@@ -3822,12 +3822,12 @@
     </row>
     <row r="678">
       <c r="A678" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="679">
       <c r="A679" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="680">
@@ -3837,12 +3837,12 @@
     </row>
     <row r="681">
       <c r="A681" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="682">
       <c r="A682" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="683">
@@ -3852,12 +3852,12 @@
     </row>
     <row r="684">
       <c r="A684" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="685">
       <c r="A685" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="686">
@@ -3877,7 +3877,7 @@
     </row>
     <row r="689">
       <c r="A689" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="690">
@@ -3887,7 +3887,7 @@
     </row>
     <row r="691">
       <c r="A691" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="692">
@@ -3897,7 +3897,7 @@
     </row>
     <row r="693">
       <c r="A693" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="694">
@@ -3912,17 +3912,17 @@
     </row>
     <row r="696">
       <c r="A696" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="697">
       <c r="A697" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="698">
       <c r="A698" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="699">
@@ -3947,7 +3947,7 @@
     </row>
     <row r="703">
       <c r="A703" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="704">
@@ -3957,27 +3957,27 @@
     </row>
     <row r="705">
       <c r="A705" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="706">
       <c r="A706" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="707">
       <c r="A707" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="708">
       <c r="A708" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="709">
       <c r="A709" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="710">
@@ -3992,7 +3992,7 @@
     </row>
     <row r="712">
       <c r="A712" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="713">
@@ -4007,7 +4007,7 @@
     </row>
     <row r="715">
       <c r="A715" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="716">
@@ -4027,12 +4027,12 @@
     </row>
     <row r="719">
       <c r="A719" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="720">
       <c r="A720" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="721">
@@ -4042,12 +4042,12 @@
     </row>
     <row r="722">
       <c r="A722" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="723">
       <c r="A723" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="724">
@@ -4057,107 +4057,107 @@
     </row>
     <row r="725">
       <c r="A725" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="726">
       <c r="A726" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="727">
       <c r="A727" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="728">
       <c r="A728" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="729">
       <c r="A729" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="730">
       <c r="A730" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="731">
       <c r="A731" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="732">
       <c r="A732" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="733">
       <c r="A733" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="734">
       <c r="A734" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="735">
       <c r="A735" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="736">
       <c r="A736" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="737">
       <c r="A737" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="738">
       <c r="A738" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="739">
       <c r="A739" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="740">
       <c r="A740" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="741">
       <c r="A741" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="742">
       <c r="A742" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="743">
       <c r="A743" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="744">
       <c r="A744" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="745">
       <c r="A745" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="746">
@@ -4242,7 +4242,7 @@
     </row>
     <row r="762">
       <c r="A762" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="763">
@@ -4252,7 +4252,7 @@
     </row>
     <row r="764">
       <c r="A764" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="765">
@@ -4267,7 +4267,7 @@
     </row>
     <row r="767">
       <c r="A767" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="768">
@@ -4277,7 +4277,7 @@
     </row>
     <row r="769">
       <c r="A769" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="770">
@@ -4287,17 +4287,17 @@
     </row>
     <row r="771">
       <c r="A771" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="772">
       <c r="A772" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="773">
       <c r="A773" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="774">
@@ -4312,12 +4312,12 @@
     </row>
     <row r="776">
       <c r="A776" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="777">
       <c r="A777" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="778">
@@ -4327,17 +4327,17 @@
     </row>
     <row r="779">
       <c r="A779" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="780">
       <c r="A780" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="781">
       <c r="A781" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="782">
@@ -4352,22 +4352,22 @@
     </row>
     <row r="784">
       <c r="A784" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="785">
       <c r="A785" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="786">
       <c r="A786" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="787">
       <c r="A787" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="788">
@@ -4382,7 +4382,7 @@
     </row>
     <row r="790">
       <c r="A790" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="791">
@@ -4392,7 +4392,7 @@
     </row>
     <row r="792">
       <c r="A792" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="793">
@@ -4417,12 +4417,12 @@
     </row>
     <row r="797">
       <c r="A797" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="798">
       <c r="A798" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="799">
@@ -4437,7 +4437,7 @@
     </row>
     <row r="801">
       <c r="A801" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="802">
@@ -4462,7 +4462,7 @@
     </row>
     <row r="806">
       <c r="A806" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="807">
@@ -4472,7 +4472,7 @@
     </row>
     <row r="808">
       <c r="A808" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="809">
@@ -4487,7 +4487,7 @@
     </row>
     <row r="811">
       <c r="A811" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="812">
@@ -4497,7 +4497,7 @@
     </row>
     <row r="813">
       <c r="A813" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="814">
@@ -4512,7 +4512,7 @@
     </row>
     <row r="816">
       <c r="A816" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="817">
@@ -4552,7 +4552,7 @@
     </row>
     <row r="824">
       <c r="A824" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="825">
@@ -4562,12 +4562,12 @@
     </row>
     <row r="826">
       <c r="A826" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="827">
       <c r="A827" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="828">
@@ -4582,12 +4582,12 @@
     </row>
     <row r="830">
       <c r="A830" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="831">
       <c r="A831" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="832">
@@ -4602,7 +4602,7 @@
     </row>
     <row r="834">
       <c r="A834" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="835">
@@ -4622,27 +4622,27 @@
     </row>
     <row r="838">
       <c r="A838" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="839">
       <c r="A839" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="840">
       <c r="A840" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="841">
       <c r="A841" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="842">
       <c r="A842" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="843">
@@ -4652,52 +4652,52 @@
     </row>
     <row r="844">
       <c r="A844" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="845">
       <c r="A845" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="846">
       <c r="A846" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="847">
       <c r="A847" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="848">
       <c r="A848" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="849">
       <c r="A849" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="850">
       <c r="A850" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="851">
       <c r="A851" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="852">
       <c r="A852" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="853">
       <c r="A853" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="854">
@@ -4707,52 +4707,52 @@
     </row>
     <row r="855">
       <c r="A855" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="856">
       <c r="A856" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="857">
       <c r="A857" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="858">
       <c r="A858" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="859">
       <c r="A859" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="860">
       <c r="A860" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="861">
       <c r="A861" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="862">
       <c r="A862" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="863">
       <c r="A863" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="864">
       <c r="A864" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="865">
@@ -4767,7 +4767,7 @@
     </row>
     <row r="867">
       <c r="A867" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="868">
@@ -4782,32 +4782,32 @@
     </row>
     <row r="870">
       <c r="A870" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="871">
       <c r="A871" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="872">
       <c r="A872" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="873">
       <c r="A873" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="874">
       <c r="A874" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="875">
       <c r="A875" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="876">
@@ -4817,17 +4817,17 @@
     </row>
     <row r="877">
       <c r="A877" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="878">
       <c r="A878" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="879">
       <c r="A879" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="880">
@@ -4837,7 +4837,7 @@
     </row>
     <row r="881">
       <c r="A881" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="882">
@@ -4847,7 +4847,7 @@
     </row>
     <row r="883">
       <c r="A883" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="884">
@@ -4857,7 +4857,7 @@
     </row>
     <row r="885">
       <c r="A885" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="886">
@@ -4872,7 +4872,7 @@
     </row>
     <row r="888">
       <c r="A888" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="889">
@@ -4887,7 +4887,7 @@
     </row>
     <row r="891">
       <c r="A891" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="892">
@@ -4897,52 +4897,52 @@
     </row>
     <row r="893">
       <c r="A893" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="894">
       <c r="A894" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="895">
       <c r="A895" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="896">
       <c r="A896" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="897">
       <c r="A897" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="898">
       <c r="A898" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="899">
       <c r="A899" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="900">
       <c r="A900" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="901">
       <c r="A901" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="902">
       <c r="A902" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="903">
@@ -4952,17 +4952,17 @@
     </row>
     <row r="904">
       <c r="A904" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="905">
       <c r="A905" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="906">
       <c r="A906" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="907">
@@ -4977,22 +4977,22 @@
     </row>
     <row r="909">
       <c r="A909" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="910">
       <c r="A910" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="911">
       <c r="A911" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="912">
       <c r="A912" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="913">
@@ -5002,7 +5002,7 @@
     </row>
     <row r="914">
       <c r="A914" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="915">
@@ -5012,7 +5012,7 @@
     </row>
     <row r="916">
       <c r="A916" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="917">
@@ -5022,7 +5022,7 @@
     </row>
     <row r="918">
       <c r="A918" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="919">
@@ -5032,22 +5032,22 @@
     </row>
     <row r="920">
       <c r="A920" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="921">
       <c r="A921" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="922">
       <c r="A922" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="923">
       <c r="A923" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="924">
@@ -5072,7 +5072,7 @@
     </row>
     <row r="928">
       <c r="A928" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="929">
@@ -5102,7 +5102,7 @@
     </row>
     <row r="934">
       <c r="A934" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="935">
@@ -5117,12 +5117,12 @@
     </row>
     <row r="937">
       <c r="A937" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="938">
       <c r="A938" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="939">
@@ -5132,7 +5132,7 @@
     </row>
     <row r="940">
       <c r="A940" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="941">
@@ -5147,7 +5147,7 @@
     </row>
     <row r="943">
       <c r="A943" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="944">
@@ -5162,7 +5162,7 @@
     </row>
     <row r="946">
       <c r="A946" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="947">
@@ -5172,12 +5172,12 @@
     </row>
     <row r="948">
       <c r="A948" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="949">
       <c r="A949" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="950">
@@ -5207,7 +5207,7 @@
     </row>
     <row r="955">
       <c r="A955" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="956">
@@ -5217,12 +5217,12 @@
     </row>
     <row r="957">
       <c r="A957" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="958">
       <c r="A958" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="959">
@@ -5232,7 +5232,7 @@
     </row>
     <row r="960">
       <c r="A960" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="961">
@@ -5242,7 +5242,7 @@
     </row>
     <row r="962">
       <c r="A962" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="963">
@@ -5252,7 +5252,7 @@
     </row>
     <row r="964">
       <c r="A964" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="965">
@@ -5267,12 +5267,12 @@
     </row>
     <row r="967">
       <c r="A967" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="968">
       <c r="A968" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="969">
@@ -5287,7 +5287,7 @@
     </row>
     <row r="971">
       <c r="A971" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="972">
@@ -5297,7 +5297,7 @@
     </row>
     <row r="973">
       <c r="A973" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="974">
@@ -5312,17 +5312,17 @@
     </row>
     <row r="976">
       <c r="A976" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="977">
       <c r="A977" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="978">
       <c r="A978" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="979">
@@ -5337,17 +5337,17 @@
     </row>
     <row r="981">
       <c r="A981" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="982">
       <c r="A982" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="983">
       <c r="A983" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="984">
@@ -5357,7 +5357,7 @@
     </row>
     <row r="985">
       <c r="A985" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="986">
@@ -5367,12 +5367,12 @@
     </row>
     <row r="987">
       <c r="A987" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="988">
       <c r="A988" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="989">
@@ -5387,17 +5387,17 @@
     </row>
     <row r="991">
       <c r="A991" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="992">
       <c r="A992" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="993">
       <c r="A993" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="994">
@@ -5407,7 +5407,7 @@
     </row>
     <row r="995">
       <c r="A995" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="996">
@@ -5427,7 +5427,7 @@
     </row>
     <row r="999">
       <c r="A999" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1000">
@@ -5437,27 +5437,27 @@
     </row>
     <row r="1001">
       <c r="A1001" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1002">
       <c r="A1002" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1003">
       <c r="A1003" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1004">
       <c r="A1004" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1005">
       <c r="A1005" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1006">
@@ -5467,27 +5467,27 @@
     </row>
     <row r="1007">
       <c r="A1007" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1008">
       <c r="A1008" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1009">
       <c r="A1009" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1010">
       <c r="A1010" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1011">
       <c r="A1011" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1012">
@@ -5502,7 +5502,7 @@
     </row>
     <row r="1014">
       <c r="A1014" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1015">
@@ -5522,52 +5522,52 @@
     </row>
     <row r="1018">
       <c r="A1018" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1019">
       <c r="A1019" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1020">
       <c r="A1020" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1021">
       <c r="A1021" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1022">
       <c r="A1022" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1023">
       <c r="A1023" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1024">
       <c r="A1024" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1025">
       <c r="A1025" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1026">
       <c r="A1026" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1027">
       <c r="A1027" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1028">
@@ -5587,12 +5587,12 @@
     </row>
     <row r="1031">
       <c r="A1031" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1032">
       <c r="A1032" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1033">
@@ -5612,17 +5612,17 @@
     </row>
     <row r="1036">
       <c r="A1036" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1037">
       <c r="A1037" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1038">
       <c r="A1038" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1039">
@@ -5632,12 +5632,12 @@
     </row>
     <row r="1040">
       <c r="A1040" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1041">
       <c r="A1041" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1042">
@@ -5657,17 +5657,17 @@
     </row>
     <row r="1045">
       <c r="A1045" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1046">
       <c r="A1046" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1047">
       <c r="A1047" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1048">
@@ -5677,7 +5677,7 @@
     </row>
     <row r="1049">
       <c r="A1049" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1050">
@@ -5687,17 +5687,17 @@
     </row>
     <row r="1051">
       <c r="A1051" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1052">
       <c r="A1052" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1053">
       <c r="A1053" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1054">
@@ -5717,37 +5717,37 @@
     </row>
     <row r="1057">
       <c r="A1057" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1058">
       <c r="A1058" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1059">
       <c r="A1059" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1060">
       <c r="A1060" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1061">
       <c r="A1061" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1062">
       <c r="A1062" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1063">
       <c r="A1063" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>